<commit_message>
updated signs on MFA data
</commit_message>
<xml_diff>
--- a/parameterization/kapp/datasets/raw_data_files/SC_MFA_flux_CENPK_batch_Rabinowitz.xlsx
+++ b/parameterization/kapp/datasets/raw_data_files/SC_MFA_flux_CENPK_batch_Rabinowitz.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ejm6426/Documents/rtRBA-main/parameterization/kapp/datasets/raw_data_files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ejm6426/Documents/scRBA/parameterization/kapp/datasets/raw_data_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81B8DC84-DC7C-1C40-AD63-A745B7E102D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D340FD77-4BC7-1847-8ECA-A61C23AFDCDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="30240" windowHeight="19500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="30240" windowHeight="19460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rxns" sheetId="1" r:id="rId1"/>
@@ -4457,6 +4457,20 @@
   </cellStyles>
   <dxfs count="3">
     <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -4485,20 +4499,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -4513,7 +4513,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{28CCC142-63E5-0C43-8DA2-635A3F61D751}" name="Table1" displayName="Table1" ref="A1:N385" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="1" tableBorderDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{28CCC142-63E5-0C43-8DA2-635A3F61D751}" name="Table1" displayName="Table1" ref="A1:N385" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
   <autoFilter ref="A1:N385" xr:uid="{28CCC142-63E5-0C43-8DA2-635A3F61D751}"/>
   <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{8826D10A-F6F0-C047-ADEC-949BD09E1179}" name="id"/>
@@ -4822,8 +4822,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N385"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="G113" sqref="G113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9402,28 +9402,28 @@
         <v>0</v>
       </c>
       <c r="G105">
-        <v>5.0278475891423033E-4</v>
+        <v>-5.0278475891423033E-4</v>
       </c>
       <c r="H105">
-        <v>5.0263767430764955E-4</v>
+        <v>-5.0263767430764955E-4</v>
       </c>
       <c r="I105">
-        <v>5.0289487430764954E-4</v>
+        <v>-5.0289487430764954E-4</v>
       </c>
       <c r="J105">
-        <v>1.815565358385475E-3</v>
+        <v>-1.815565358385475E-3</v>
       </c>
       <c r="K105">
-        <v>1.815034233064499E-3</v>
+        <v>-1.815034233064499E-3</v>
       </c>
       <c r="L105">
-        <v>1.8159629871722909E-3</v>
+        <v>-1.8159629871722909E-3</v>
       </c>
       <c r="M105">
-        <v>5.0284937531644913E-4</v>
+        <v>-5.0284937531644913E-4</v>
       </c>
       <c r="N105">
-        <v>1.815805243158865E-3</v>
+        <v>-1.815805243158865E-3</v>
       </c>
     </row>
     <row r="106" spans="1:14" x14ac:dyDescent="0.2">
@@ -9484,28 +9484,28 @@
         <v>0</v>
       </c>
       <c r="G107">
-        <v>4.4570596846566949E-5</v>
+        <v>-4.4570596846566949E-5</v>
       </c>
       <c r="H107">
-        <v>4.4557305498500819E-5</v>
+        <v>-4.4557305498500819E-5</v>
       </c>
       <c r="I107">
-        <v>4.4580105498500808E-5</v>
+        <v>-4.4580105498500808E-5</v>
       </c>
       <c r="J107">
-        <v>1.6094527569201049E-4</v>
+        <v>-1.6094527569201049E-4</v>
       </c>
       <c r="K107">
-        <v>1.6089728038052331E-4</v>
+        <v>-1.6089728038052331E-4</v>
       </c>
       <c r="L107">
-        <v>1.6097961161558411E-4</v>
+        <v>-1.6097961161558411E-4</v>
       </c>
       <c r="M107">
-        <v>4.46E-5</v>
+        <v>-4.46E-5</v>
       </c>
       <c r="N107">
-        <v>1.610520323186652E-4</v>
+        <v>-1.610520323186652E-4</v>
       </c>
     </row>
     <row r="108" spans="1:14" x14ac:dyDescent="0.2">
@@ -9566,28 +9566,28 @@
         <v>0</v>
       </c>
       <c r="G109">
-        <v>2.5958981831323289E-4</v>
+        <v>-2.5958981831323289E-4</v>
       </c>
       <c r="H109">
-        <v>2.5952676185091698E-4</v>
+        <v>-2.5952676185091698E-4</v>
       </c>
       <c r="I109">
-        <v>2.59659561850917E-4</v>
+        <v>-2.59659561850917E-4</v>
       </c>
       <c r="J109">
-        <v>9.3738378732256703E-4</v>
+        <v>-9.3738378732256703E-4</v>
       </c>
       <c r="K109">
-        <v>9.3715608923392502E-4</v>
+        <v>-9.3715608923392502E-4</v>
       </c>
       <c r="L109">
-        <v>9.3763563256796364E-4</v>
+        <v>-9.3763563256796364E-4</v>
       </c>
       <c r="M109">
-        <v>2.5963606937023503E-4</v>
+        <v>-2.5963606937023503E-4</v>
       </c>
       <c r="N109">
-        <v>9.3755418464812302E-4</v>
+        <v>-9.3755418464812302E-4</v>
       </c>
     </row>
     <row r="110" spans="1:14" x14ac:dyDescent="0.2">
@@ -9607,28 +9607,28 @@
         <v>0</v>
       </c>
       <c r="G110">
-        <v>27.693013451266829</v>
+        <v>-27.693013451266829</v>
       </c>
       <c r="H110">
-        <v>27.692913451266829</v>
+        <v>-27.692913451266829</v>
       </c>
       <c r="I110">
-        <v>27.693113451266829</v>
+        <v>-27.693113451266829</v>
       </c>
       <c r="J110">
-        <v>100</v>
+        <v>-100</v>
       </c>
       <c r="K110">
-        <v>99.999638898091831</v>
+        <v>-99.999638898091831</v>
       </c>
       <c r="L110">
-        <v>100.0003611019082</v>
+        <v>-100.0003611019082</v>
       </c>
       <c r="M110">
-        <v>27.6929135</v>
+        <v>-27.6929135</v>
       </c>
       <c r="N110">
-        <v>100</v>
+        <v>-100</v>
       </c>
     </row>
     <row r="111" spans="1:14" x14ac:dyDescent="0.2">
@@ -9730,28 +9730,28 @@
         <v>0</v>
       </c>
       <c r="G113">
-        <v>0.23599910635110469</v>
+        <v>-0.23599910635110469</v>
       </c>
       <c r="H113">
-        <v>0.23593874968570189</v>
+        <v>-0.23593874968570189</v>
       </c>
       <c r="I113">
-        <v>0.2360594796857019</v>
+        <v>-0.2360594796857019</v>
       </c>
       <c r="J113">
-        <v>0.85219727627839226</v>
+        <v>-0.85219727627839226</v>
       </c>
       <c r="K113">
-        <v>0.85197932720792002</v>
+        <v>-0.85197932720792002</v>
       </c>
       <c r="L113">
-        <v>0.85241528554164359</v>
+        <v>-0.85241528554164359</v>
       </c>
       <c r="M113">
-        <v>0.23603812240262401</v>
+        <v>-0.23603812240262401</v>
       </c>
       <c r="N113">
-        <v>0.8523412403054812</v>
+        <v>-0.8523412403054812</v>
       </c>
     </row>
     <row r="114" spans="1:14" x14ac:dyDescent="0.2">
@@ -9771,28 +9771,28 @@
         <v>0</v>
       </c>
       <c r="G114">
-        <v>2.486738260970427E-2</v>
+        <v>-2.486738260970427E-2</v>
       </c>
       <c r="H114">
-        <v>2.4861022200378429E-2</v>
+        <v>-2.4861022200378429E-2</v>
       </c>
       <c r="I114">
-        <v>2.4873743600378431E-2</v>
+        <v>-2.4873743600378431E-2</v>
       </c>
       <c r="J114">
-        <v>8.979659311351218E-2</v>
+        <v>-8.979659311351218E-2</v>
       </c>
       <c r="K114">
-        <v>8.9773625554069675E-2</v>
+        <v>-8.9773625554069675E-2</v>
       </c>
       <c r="L114">
-        <v>8.9819562772214562E-2</v>
+        <v>-8.9819562772214562E-2</v>
       </c>
       <c r="M114">
-        <v>2.487149316932611E-2</v>
+        <v>-2.487149316932611E-2</v>
       </c>
       <c r="N114">
-        <v>8.9811760576676433E-2</v>
+        <v>-8.9811760576676433E-2</v>
       </c>
     </row>
     <row r="115" spans="1:14" x14ac:dyDescent="0.2">
@@ -9812,28 +9812,28 @@
         <v>0</v>
       </c>
       <c r="G115">
-        <v>3.6748470144450228E-5</v>
+        <v>-3.6748470144450228E-5</v>
       </c>
       <c r="H115">
-        <v>3.6740234358412949E-5</v>
+        <v>-3.6740234358412949E-5</v>
       </c>
       <c r="I115">
-        <v>3.675903435841295E-5</v>
+        <v>-3.675903435841295E-5</v>
       </c>
       <c r="J115">
-        <v>1.3269942691184139E-4</v>
+        <v>-1.3269942691184139E-4</v>
       </c>
       <c r="K115">
-        <v>1.3266968733130859E-4</v>
+        <v>-1.3266968733130859E-4</v>
       </c>
       <c r="L115">
-        <v>1.3273757449004309E-4</v>
+        <v>-1.3273757449004309E-4</v>
       </c>
       <c r="M115">
-        <v>3.6755708615665803E-5</v>
+        <v>-3.6755708615665803E-5</v>
       </c>
       <c r="N115">
-        <v>1.327260442122343E-4</v>
+        <v>-1.327260442122343E-4</v>
       </c>
     </row>
     <row r="116" spans="1:14" x14ac:dyDescent="0.2">
@@ -9853,28 +9853,28 @@
         <v>0</v>
       </c>
       <c r="G116">
-        <v>3.1109889598980391</v>
+        <v>-3.1109889598980391</v>
       </c>
       <c r="H116">
-        <v>3.1101933705520501</v>
+        <v>-3.1101933705520501</v>
       </c>
       <c r="I116">
-        <v>3.1117848531436469</v>
+        <v>-3.1117848531436469</v>
       </c>
       <c r="J116">
-        <v>11.23384049689156</v>
+        <v>-11.23384049689156</v>
       </c>
       <c r="K116">
-        <v>11.230967608582059</v>
+        <v>-11.230967608582059</v>
       </c>
       <c r="L116">
-        <v>11.23671448258837</v>
+        <v>-11.23671448258837</v>
       </c>
       <c r="M116">
-        <v>3.111503289477823</v>
+        <v>-3.111503289477823</v>
       </c>
       <c r="N116">
-        <v>11.23573830351156</v>
+        <v>-11.23573830351156</v>
       </c>
     </row>
     <row r="117" spans="1:14" x14ac:dyDescent="0.2">
@@ -9894,28 +9894,28 @@
         <v>0</v>
       </c>
       <c r="G117">
-        <v>5.6069593885133298</v>
+        <v>-5.6069593885133298</v>
       </c>
       <c r="H117">
-        <v>5.60685938851333</v>
+        <v>-5.60685938851333</v>
       </c>
       <c r="I117">
-        <v>5.6070593885133304</v>
+        <v>-5.6070593885133304</v>
       </c>
       <c r="J117">
-        <v>20.246837341773059</v>
+        <v>-20.246837341773059</v>
       </c>
       <c r="K117">
-        <v>20.246476239864901</v>
+        <v>-20.246476239864901</v>
       </c>
       <c r="L117">
-        <v>20.247198443681221</v>
+        <v>-20.247198443681221</v>
       </c>
       <c r="M117">
-        <v>5.6068594000000003</v>
+        <v>-5.6068594000000003</v>
       </c>
       <c r="N117">
-        <v>20.2465493563904</v>
+        <v>-20.2465493563904</v>
       </c>
     </row>
     <row r="118" spans="1:14" x14ac:dyDescent="0.2">
@@ -9935,28 +9935,28 @@
         <v>0</v>
       </c>
       <c r="G118">
-        <v>0.2269148953559742</v>
+        <v>-0.2269148953559742</v>
       </c>
       <c r="H118">
-        <v>0.22685682214492919</v>
+        <v>-0.22685682214492919</v>
       </c>
       <c r="I118">
-        <v>0.22697286015901369</v>
+        <v>-0.22697286015901369</v>
       </c>
       <c r="J118">
-        <v>0.81939401703354142</v>
+        <v>-0.81939401703354142</v>
       </c>
       <c r="K118">
-        <v>0.81918431356032695</v>
+        <v>-0.81918431356032695</v>
       </c>
       <c r="L118">
-        <v>0.81960332904337929</v>
+        <v>-0.81960332904337929</v>
       </c>
       <c r="M118">
-        <v>0.22695242404720689</v>
+        <v>-0.22695242404720689</v>
       </c>
       <c r="N118">
-        <v>0.81953249175897269</v>
+        <v>-0.81953249175897269</v>
       </c>
     </row>
     <row r="119" spans="1:14" x14ac:dyDescent="0.2">
@@ -9976,28 +9976,28 @@
         <v>0</v>
       </c>
       <c r="G119">
-        <v>3.5794517105617207E-2</v>
+        <v>-3.5794517105617207E-2</v>
       </c>
       <c r="H119">
-        <v>3.578537911865122E-2</v>
+        <v>-3.578537911865122E-2</v>
       </c>
       <c r="I119">
-        <v>3.5803690518651218E-2</v>
+        <v>-3.5803690518651218E-2</v>
       </c>
       <c r="J119">
-        <v>0.12925468428564879</v>
+        <v>-0.12925468428564879</v>
       </c>
       <c r="K119">
-        <v>0.1292216868403471</v>
+        <v>-0.1292216868403471</v>
       </c>
       <c r="L119">
-        <v>0.12928780965515821</v>
+        <v>-0.12928780965515821</v>
       </c>
       <c r="M119">
-        <v>3.5800451209835243E-2</v>
+        <v>-3.5800451209835243E-2</v>
       </c>
       <c r="N119">
-        <v>0.12927657904190989</v>
+        <v>-0.12927657904190989</v>
       </c>
     </row>
     <row r="120" spans="1:14" x14ac:dyDescent="0.2">
@@ -10017,28 +10017,28 @@
         <v>0</v>
       </c>
       <c r="G120">
-        <v>6.161713331952934E-4</v>
+        <v>-6.161713331952934E-4</v>
       </c>
       <c r="H120">
-        <v>6.1598520583892348E-4</v>
+        <v>-6.1598520583892348E-4</v>
       </c>
       <c r="I120">
-        <v>6.1630040583892352E-4</v>
+        <v>-6.1630040583892352E-4</v>
       </c>
       <c r="J120">
-        <v>2.225006441713574E-3</v>
+        <v>-2.225006441713574E-3</v>
       </c>
       <c r="K120">
-        <v>2.224334332278111E-3</v>
+        <v>-2.224334332278111E-3</v>
       </c>
       <c r="L120">
-        <v>2.2254725254926369E-3</v>
+        <v>-2.2254725254926369E-3</v>
       </c>
       <c r="M120">
-        <v>6.1624464657754569E-4</v>
+        <v>-6.1624464657754569E-4</v>
       </c>
       <c r="N120">
-        <v>2.225279209345545E-3</v>
+        <v>-2.225279209345545E-3</v>
       </c>
     </row>
     <row r="121" spans="1:14" x14ac:dyDescent="0.2">

</xml_diff>